<commit_message>
began new folder for the non-ARC transients
</commit_message>
<xml_diff>
--- a/BnB/worths.xlsx
+++ b/BnB/worths.xlsx
@@ -140,14 +140,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000E+00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -199,46 +192,46 @@
   </borders>
   <cellStyleXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="35">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1647,11 +1640,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-151832224"/>
-        <c:axId val="-151834544"/>
+        <c:axId val="1578963824"/>
+        <c:axId val="1578930752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-151832224"/>
+        <c:axId val="1578963824"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1707,12 +1700,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-151834544"/>
+        <c:crossAx val="1578930752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-151834544"/>
+        <c:axId val="1578930752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1768,7 +1761,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-151832224"/>
+        <c:crossAx val="1578963824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3218,11 +3211,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-152147424"/>
-        <c:axId val="-125703904"/>
+        <c:axId val="1581613712"/>
+        <c:axId val="1581615488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-152147424"/>
+        <c:axId val="1581613712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3242,6 +3235,7 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -3278,12 +3272,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-125703904"/>
+        <c:crossAx val="1581615488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-125703904"/>
+        <c:axId val="1581615488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3340,7 +3334,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-152147424"/>
+        <c:crossAx val="1581613712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4781,11 +4775,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-125034144"/>
-        <c:axId val="-179784832"/>
+        <c:axId val="1581314720"/>
+        <c:axId val="1578432976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-125034144"/>
+        <c:axId val="1581314720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4841,12 +4835,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-179784832"/>
+        <c:crossAx val="1578432976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-179784832"/>
+        <c:axId val="1578432976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4902,7 +4896,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-125034144"/>
+        <c:crossAx val="1581314720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6343,11 +6337,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-121499904"/>
-        <c:axId val="-121501680"/>
+        <c:axId val="1581651056"/>
+        <c:axId val="1581653808"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-121499904"/>
+        <c:axId val="1581651056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6403,12 +6397,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-121501680"/>
+        <c:crossAx val="1581653808"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-121501680"/>
+        <c:axId val="1581653808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6464,7 +6458,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-121499904"/>
+        <c:crossAx val="1581651056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -7905,11 +7899,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-120305776"/>
-        <c:axId val="-151888064"/>
+        <c:axId val="1581704224"/>
+        <c:axId val="1581706976"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-120305776"/>
+        <c:axId val="1581704224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7966,12 +7960,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-151888064"/>
+        <c:crossAx val="1581706976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-151888064"/>
+        <c:axId val="1581706976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8027,7 +8021,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-120305776"/>
+        <c:crossAx val="1581704224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -9468,11 +9462,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-118947568"/>
-        <c:axId val="-118949344"/>
+        <c:axId val="1581748736"/>
+        <c:axId val="1581751488"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-118947568"/>
+        <c:axId val="1581748736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9528,12 +9522,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-118949344"/>
+        <c:crossAx val="1581751488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-118949344"/>
+        <c:axId val="1581751488"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -9589,7 +9583,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-118947568"/>
+        <c:crossAx val="1581748736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -13466,8 +13460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55:H80"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15570,15 +15564,15 @@
         <v>0.125</v>
       </c>
       <c r="B30" s="2">
-        <f>A3</f>
+        <f t="shared" ref="B30:B53" si="0">A3</f>
         <v>2.6841999999999999E-10</v>
       </c>
       <c r="C30" s="2">
-        <f>AVERAGE(D3,G3)</f>
+        <f t="shared" ref="C30:C53" si="1">AVERAGE(D3,G3)</f>
         <v>8.8369999999999996E-10</v>
       </c>
       <c r="D30" s="2">
-        <f>AVERAGE(J4,M3,P3)</f>
+        <f t="shared" ref="D30:D53" si="2">AVERAGE(J4,M3,P3)</f>
         <v>-3.3083333333333322E-11</v>
       </c>
       <c r="E30" s="2">
@@ -15590,11 +15584,11 @@
         <v>0</v>
       </c>
       <c r="G30" s="2">
-        <f>A3</f>
+        <f t="shared" ref="G30:G53" si="3">A3</f>
         <v>2.6841999999999999E-10</v>
       </c>
       <c r="H30" s="2">
-        <f>D3</f>
+        <f t="shared" ref="H30:H53" si="4">D3</f>
         <v>1.5197E-9</v>
       </c>
     </row>
@@ -15603,19 +15597,19 @@
         <v>0.25</v>
       </c>
       <c r="B31" s="2">
-        <f>A4</f>
+        <f t="shared" si="0"/>
         <v>-2.7420999999999998E-10</v>
       </c>
       <c r="C31" s="2">
-        <f>AVERAGE(D4,G4)</f>
+        <f t="shared" si="1"/>
         <v>-1.1389650000000001E-9</v>
       </c>
       <c r="D31" s="2">
-        <f>AVERAGE(J5,M4,P4)</f>
+        <f t="shared" si="2"/>
         <v>2.8853066666666665E-9</v>
       </c>
       <c r="E31" s="2">
-        <f>AVERAGE(S4,V4,Y4,AB4, AE4, AH4)</f>
+        <f t="shared" ref="E30:E53" si="5">AVERAGE(S4,V4,Y4,AB4, AE4, AH4)</f>
         <v>1.1181500000000002E-11</v>
       </c>
       <c r="F31" s="2">
@@ -15623,11 +15617,11 @@
         <v>0</v>
       </c>
       <c r="G31" s="2">
-        <f>A4</f>
+        <f t="shared" si="3"/>
         <v>-2.7420999999999998E-10</v>
       </c>
       <c r="H31" s="2">
-        <f>D4</f>
+        <f t="shared" si="4"/>
         <v>-1.5616000000000001E-9</v>
       </c>
     </row>
@@ -15636,19 +15630,19 @@
         <v>0.375</v>
       </c>
       <c r="B32" s="2">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>-1.6633E-9</v>
       </c>
       <c r="C32" s="2">
-        <f>AVERAGE(D5,G5)</f>
+        <f t="shared" si="1"/>
         <v>-1.7155700000000001E-9</v>
       </c>
       <c r="D32" s="2">
-        <f>AVERAGE(J6,M5,P5)</f>
+        <f t="shared" si="2"/>
         <v>2.8097699999999999E-9</v>
       </c>
       <c r="E32" s="2">
-        <f>AVERAGE(S5,V5,Y5,AB5, AE5, AH5)</f>
+        <f t="shared" si="5"/>
         <v>2.6801103333333332E-10</v>
       </c>
       <c r="F32" s="2">
@@ -15656,11 +15650,11 @@
         <v>0</v>
       </c>
       <c r="G32" s="2">
-        <f>A5</f>
+        <f t="shared" si="3"/>
         <v>-1.6633E-9</v>
       </c>
       <c r="H32" s="2">
-        <f>D5</f>
+        <f t="shared" si="4"/>
         <v>-3.6921000000000001E-9</v>
       </c>
     </row>
@@ -15669,19 +15663,19 @@
         <v>0.5</v>
       </c>
       <c r="B33" s="2">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>-6.2551E-9</v>
       </c>
       <c r="C33" s="2">
-        <f>AVERAGE(D6,G6)</f>
+        <f t="shared" si="1"/>
         <v>1.1671549999999999E-8</v>
       </c>
       <c r="D33" s="2">
-        <f>AVERAGE(J7,M6,P6)</f>
+        <f t="shared" si="2"/>
         <v>3.0638700000000004E-8</v>
       </c>
       <c r="E33" s="2">
-        <f>AVERAGE(S6,V6,Y6,AB6, AE6, AH6)</f>
+        <f t="shared" si="5"/>
         <v>2.2966000000000004E-10</v>
       </c>
       <c r="F33" s="2">
@@ -15689,11 +15683,11 @@
         <v>0</v>
       </c>
       <c r="G33" s="2">
-        <f>A6</f>
+        <f t="shared" si="3"/>
         <v>-6.2551E-9</v>
       </c>
       <c r="H33" s="2">
-        <f>D6</f>
+        <f t="shared" si="4"/>
         <v>1.6961E-9</v>
       </c>
     </row>
@@ -15702,19 +15696,19 @@
         <v>0.625</v>
       </c>
       <c r="B34" s="2">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>-1.5040999999999999E-8</v>
       </c>
       <c r="C34" s="2">
-        <f>AVERAGE(D7,G7)</f>
+        <f t="shared" si="1"/>
         <v>3.5088000000000003E-8</v>
       </c>
       <c r="D34" s="2">
-        <f>AVERAGE(J8,M7,P7)</f>
+        <f t="shared" si="2"/>
         <v>1.4796433333333333E-7</v>
       </c>
       <c r="E34" s="2">
-        <f>AVERAGE(S7,V7,Y7,AB7, AE7, AH7)</f>
+        <f t="shared" si="5"/>
         <v>7.6993999999999993E-10</v>
       </c>
       <c r="F34" s="2">
@@ -15722,11 +15716,11 @@
         <v>0</v>
       </c>
       <c r="G34" s="2">
-        <f>A7</f>
+        <f t="shared" si="3"/>
         <v>-1.5040999999999999E-8</v>
       </c>
       <c r="H34" s="2">
-        <f>D7</f>
+        <f t="shared" si="4"/>
         <v>1.7149E-8</v>
       </c>
     </row>
@@ -15735,19 +15729,19 @@
         <v>0.75</v>
       </c>
       <c r="B35" s="2">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>-2.1025000000000001E-8</v>
       </c>
       <c r="C35" s="2">
-        <f>AVERAGE(D8,G8)</f>
+        <f t="shared" si="1"/>
         <v>2.1829999999999999E-7</v>
       </c>
       <c r="D35" s="2">
-        <f>AVERAGE(J9,M8,P8)</f>
+        <f t="shared" si="2"/>
         <v>4.6253400000000006E-7</v>
       </c>
       <c r="E35" s="2">
-        <f>AVERAGE(S8,V8,Y8,AB8, AE8, AH8)</f>
+        <f t="shared" si="5"/>
         <v>4.0840533333333322E-9</v>
       </c>
       <c r="F35" s="2">
@@ -15755,11 +15749,11 @@
         <v>0</v>
       </c>
       <c r="G35" s="2">
-        <f>A8</f>
+        <f t="shared" si="3"/>
         <v>-2.1025000000000001E-8</v>
       </c>
       <c r="H35" s="2">
-        <f>D8</f>
+        <f t="shared" si="4"/>
         <v>1.4158E-7</v>
       </c>
     </row>
@@ -15768,19 +15762,19 @@
         <v>0.875</v>
       </c>
       <c r="B36" s="2">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>-2.7599000000000001E-8</v>
       </c>
       <c r="C36" s="2">
-        <f>AVERAGE(D9,G9)</f>
+        <f t="shared" si="1"/>
         <v>8.190300000000001E-7</v>
       </c>
       <c r="D36" s="2">
-        <f>AVERAGE(J10,M9,P9)</f>
+        <f t="shared" si="2"/>
         <v>1.0119133333333335E-6</v>
       </c>
       <c r="E36" s="2">
-        <f>AVERAGE(S9,V9,Y9,AB9, AE9, AH9)</f>
+        <f t="shared" si="5"/>
         <v>1.5032671666666669E-8</v>
       </c>
       <c r="F36" s="2">
@@ -15788,11 +15782,11 @@
         <v>0</v>
       </c>
       <c r="G36" s="2">
-        <f>A9</f>
+        <f t="shared" si="3"/>
         <v>-2.7599000000000001E-8</v>
       </c>
       <c r="H36" s="2">
-        <f>D9</f>
+        <f t="shared" si="4"/>
         <v>5.7716000000000001E-7</v>
       </c>
     </row>
@@ -15801,19 +15795,19 @@
         <v>1</v>
       </c>
       <c r="B37" s="2">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>-5.9796000000000002E-8</v>
       </c>
       <c r="C37" s="2">
-        <f>AVERAGE(D10,G10)</f>
+        <f t="shared" si="1"/>
         <v>1.5402500000000002E-6</v>
       </c>
       <c r="D37" s="2">
-        <f>AVERAGE(J11,M10,P10)</f>
+        <f t="shared" si="2"/>
         <v>1.8043433333333333E-6</v>
       </c>
       <c r="E37" s="2">
-        <f>AVERAGE(S10,V10,Y10,AB10, AE10, AH10)</f>
+        <f t="shared" si="5"/>
         <v>1.5545828333333336E-8</v>
       </c>
       <c r="F37" s="2">
@@ -15821,11 +15815,11 @@
         <v>0</v>
       </c>
       <c r="G37" s="2">
-        <f>A10</f>
+        <f t="shared" si="3"/>
         <v>-5.9796000000000002E-8</v>
       </c>
       <c r="H37" s="2">
-        <f>D10</f>
+        <f t="shared" si="4"/>
         <v>1.0937E-6</v>
       </c>
     </row>
@@ -15834,19 +15828,19 @@
         <v>1.125</v>
       </c>
       <c r="B38" s="2">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>2.0947999999999999E-7</v>
       </c>
       <c r="C38" s="2">
-        <f>AVERAGE(D11,G11)</f>
+        <f t="shared" si="1"/>
         <v>3.7692500000000004E-6</v>
       </c>
       <c r="D38" s="2">
-        <f>AVERAGE(J12,M11,P11)</f>
+        <f t="shared" si="2"/>
         <v>2.5608833333333332E-6</v>
       </c>
       <c r="E38" s="2">
-        <f>AVERAGE(S11,V11,Y11,AB11, AE11, AH11)</f>
+        <f t="shared" si="5"/>
         <v>5.7512363333333331E-8</v>
       </c>
       <c r="F38" s="2">
@@ -15854,11 +15848,11 @@
         <v>0</v>
       </c>
       <c r="G38" s="2">
-        <f>A11</f>
+        <f t="shared" si="3"/>
         <v>2.0947999999999999E-7</v>
       </c>
       <c r="H38" s="2">
-        <f>D11</f>
+        <f t="shared" si="4"/>
         <v>3.2571000000000001E-6</v>
       </c>
     </row>
@@ -15867,19 +15861,19 @@
         <v>1.25</v>
       </c>
       <c r="B39" s="2">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>1.8234999999999999E-7</v>
       </c>
       <c r="C39" s="2">
-        <f>AVERAGE(D12,G12)</f>
+        <f t="shared" si="1"/>
         <v>5.1181999999999995E-6</v>
       </c>
       <c r="D39" s="2">
-        <f>AVERAGE(J13,M12,P12)</f>
+        <f t="shared" si="2"/>
         <v>3.1416666666666669E-6</v>
       </c>
       <c r="E39" s="2">
-        <f>AVERAGE(S12,V12,Y12,AB12, AE12, AH12)</f>
+        <f t="shared" si="5"/>
         <v>7.3530855000000002E-8</v>
       </c>
       <c r="F39" s="2">
@@ -15887,11 +15881,11 @@
         <v>0</v>
       </c>
       <c r="G39" s="2">
-        <f>A12</f>
+        <f t="shared" si="3"/>
         <v>1.8234999999999999E-7</v>
       </c>
       <c r="H39" s="2">
-        <f>D12</f>
+        <f t="shared" si="4"/>
         <v>4.5622000000000001E-6</v>
       </c>
     </row>
@@ -15900,19 +15894,19 @@
         <v>1.375</v>
       </c>
       <c r="B40" s="2">
-        <f>A13</f>
+        <f t="shared" si="0"/>
         <v>5.8199000000000004E-7</v>
       </c>
       <c r="C40" s="2">
-        <f>AVERAGE(D13,G13)</f>
+        <f t="shared" si="1"/>
         <v>6.5357E-6</v>
       </c>
       <c r="D40" s="2">
-        <f>AVERAGE(J14,M13,P13)</f>
+        <f t="shared" si="2"/>
         <v>3.3061E-6</v>
       </c>
       <c r="E40" s="2">
-        <f>AVERAGE(S13,V13,Y13,AB13, AE13, AH13)</f>
+        <f t="shared" si="5"/>
         <v>1.1422178333333332E-7</v>
       </c>
       <c r="F40" s="2">
@@ -15920,11 +15914,11 @@
         <v>0</v>
       </c>
       <c r="G40" s="2">
-        <f>A13</f>
+        <f t="shared" si="3"/>
         <v>5.8199000000000004E-7</v>
       </c>
       <c r="H40" s="2">
-        <f>D13</f>
+        <f t="shared" si="4"/>
         <v>6.2097E-6</v>
       </c>
     </row>
@@ -15933,19 +15927,19 @@
         <v>1.5</v>
       </c>
       <c r="B41" s="2">
-        <f>A14</f>
+        <f t="shared" si="0"/>
         <v>9.1795000000000004E-7</v>
       </c>
       <c r="C41" s="2">
-        <f>AVERAGE(D14,G14)</f>
+        <f t="shared" si="1"/>
         <v>7.2915999999999998E-6</v>
       </c>
       <c r="D41" s="2">
-        <f>AVERAGE(J15,M14,P14)</f>
+        <f t="shared" si="2"/>
         <v>3.4422666666666671E-6</v>
       </c>
       <c r="E41" s="2">
-        <f>AVERAGE(S14,V14,Y14,AB14, AE14, AH14)</f>
+        <f t="shared" si="5"/>
         <v>1.6191960166666667E-7</v>
       </c>
       <c r="F41" s="2">
@@ -15953,11 +15947,11 @@
         <v>0</v>
       </c>
       <c r="G41" s="2">
-        <f>A14</f>
+        <f t="shared" si="3"/>
         <v>9.1795000000000004E-7</v>
       </c>
       <c r="H41" s="2">
-        <f>D14</f>
+        <f t="shared" si="4"/>
         <v>7.3077000000000004E-6</v>
       </c>
     </row>
@@ -15966,19 +15960,19 @@
         <v>1.625</v>
       </c>
       <c r="B42" s="2">
-        <f>A15</f>
+        <f t="shared" si="0"/>
         <v>9.6121999999999992E-7</v>
       </c>
       <c r="C42" s="2">
-        <f>AVERAGE(D15,G15)</f>
+        <f t="shared" si="1"/>
         <v>7.85645E-6</v>
       </c>
       <c r="D42" s="2">
-        <f>AVERAGE(J16,M15,P15)</f>
+        <f t="shared" si="2"/>
         <v>3.5555333333333335E-6</v>
       </c>
       <c r="E42" s="2">
-        <f>AVERAGE(S15,V15,Y15,AB15, AE15, AH15)</f>
+        <f t="shared" si="5"/>
         <v>1.3882756666666667E-7</v>
       </c>
       <c r="F42" s="2">
@@ -15986,11 +15980,11 @@
         <v>0</v>
       </c>
       <c r="G42" s="2">
-        <f>A15</f>
+        <f t="shared" si="3"/>
         <v>9.6121999999999992E-7</v>
       </c>
       <c r="H42" s="2">
-        <f>D15</f>
+        <f t="shared" si="4"/>
         <v>7.8735000000000001E-6</v>
       </c>
     </row>
@@ -15999,19 +15993,19 @@
         <v>1.75</v>
       </c>
       <c r="B43" s="2">
-        <f>A16</f>
+        <f t="shared" si="0"/>
         <v>5.9976000000000002E-7</v>
       </c>
       <c r="C43" s="2">
-        <f>AVERAGE(D16,G16)</f>
+        <f t="shared" si="1"/>
         <v>7.2826000000000004E-6</v>
       </c>
       <c r="D43" s="2">
-        <f>AVERAGE(J17,M16,P16)</f>
+        <f t="shared" si="2"/>
         <v>3.4182999999999995E-6</v>
       </c>
       <c r="E43" s="2">
-        <f>AVERAGE(S16,V16,Y16,AB16, AE16, AH16)</f>
+        <f t="shared" si="5"/>
         <v>1.4057948000000003E-7</v>
       </c>
       <c r="F43" s="2">
@@ -16019,11 +16013,11 @@
         <v>0</v>
       </c>
       <c r="G43" s="2">
-        <f>A16</f>
+        <f t="shared" si="3"/>
         <v>5.9976000000000002E-7</v>
       </c>
       <c r="H43" s="2">
-        <f>D16</f>
+        <f t="shared" si="4"/>
         <v>6.9383000000000001E-6</v>
       </c>
     </row>
@@ -16032,19 +16026,19 @@
         <v>1.875</v>
       </c>
       <c r="B44" s="2">
-        <f>A17</f>
+        <f t="shared" si="0"/>
         <v>6.8711999999999997E-7</v>
       </c>
       <c r="C44" s="2">
-        <f>AVERAGE(D17,G17)</f>
+        <f t="shared" si="1"/>
         <v>6.5226E-6</v>
       </c>
       <c r="D44" s="2">
-        <f>AVERAGE(J18,M17,P17)</f>
+        <f t="shared" si="2"/>
         <v>3.1169666666666661E-6</v>
       </c>
       <c r="E44" s="2">
-        <f>AVERAGE(S17,V17,Y17,AB17, AE17, AH17)</f>
+        <f t="shared" si="5"/>
         <v>1.0865786333333335E-7</v>
       </c>
       <c r="F44" s="2">
@@ -16052,11 +16046,11 @@
         <v>0</v>
       </c>
       <c r="G44" s="2">
-        <f>A17</f>
+        <f t="shared" si="3"/>
         <v>6.8711999999999997E-7</v>
       </c>
       <c r="H44" s="2">
-        <f>D17</f>
+        <f t="shared" si="4"/>
         <v>6.3477000000000002E-6</v>
       </c>
     </row>
@@ -16065,19 +16059,19 @@
         <v>2</v>
       </c>
       <c r="B45" s="2">
-        <f>A18</f>
+        <f t="shared" si="0"/>
         <v>3.8823999999999999E-7</v>
       </c>
       <c r="C45" s="2">
-        <f>AVERAGE(D18,G18)</f>
+        <f t="shared" si="1"/>
         <v>5.2111E-6</v>
       </c>
       <c r="D45" s="2">
-        <f>AVERAGE(J19,M18,P18)</f>
+        <f t="shared" si="2"/>
         <v>2.5478666666666664E-6</v>
       </c>
       <c r="E45" s="2">
-        <f>AVERAGE(S18,V18,Y18,AB18, AE18, AH18)</f>
+        <f t="shared" si="5"/>
         <v>8.9919694999999993E-8</v>
       </c>
       <c r="F45" s="2">
@@ -16085,11 +16079,11 @@
         <v>0</v>
       </c>
       <c r="G45" s="2">
-        <f>A18</f>
+        <f t="shared" si="3"/>
         <v>3.8823999999999999E-7</v>
       </c>
       <c r="H45" s="2">
-        <f>D18</f>
+        <f t="shared" si="4"/>
         <v>4.8539000000000002E-6</v>
       </c>
     </row>
@@ -16098,19 +16092,19 @@
         <v>2.125</v>
       </c>
       <c r="B46" s="2">
-        <f>A19</f>
+        <f t="shared" si="0"/>
         <v>8.9815000000000001E-8</v>
       </c>
       <c r="C46" s="2">
-        <f>AVERAGE(D19,G19)</f>
+        <f t="shared" si="1"/>
         <v>3.3021000000000001E-6</v>
       </c>
       <c r="D46" s="2">
-        <f>AVERAGE(J20,M19,P19)</f>
+        <f t="shared" si="2"/>
         <v>1.8064233333333335E-6</v>
       </c>
       <c r="E46" s="2">
-        <f>AVERAGE(S19,V19,Y19,AB19, AE19, AH19)</f>
+        <f t="shared" si="5"/>
         <v>3.5738134999999999E-8</v>
       </c>
       <c r="F46" s="2">
@@ -16118,11 +16112,11 @@
         <v>0</v>
       </c>
       <c r="G46" s="2">
-        <f>A19</f>
+        <f t="shared" si="3"/>
         <v>8.9815000000000001E-8</v>
       </c>
       <c r="H46" s="2">
-        <f>D19</f>
+        <f t="shared" si="4"/>
         <v>2.5527000000000001E-6</v>
       </c>
     </row>
@@ -16131,19 +16125,19 @@
         <v>2.25</v>
       </c>
       <c r="B47" s="2">
-        <f>A20</f>
+        <f t="shared" si="0"/>
         <v>4.6621999999999999E-9</v>
       </c>
       <c r="C47" s="2">
-        <f>AVERAGE(D20,G20)</f>
+        <f t="shared" si="1"/>
         <v>2.0847000000000001E-6</v>
       </c>
       <c r="D47" s="2">
-        <f>AVERAGE(J21,M20,P20)</f>
+        <f t="shared" si="2"/>
         <v>1.0513033333333332E-6</v>
       </c>
       <c r="E47" s="2">
-        <f>AVERAGE(S20,V20,Y20,AB20, AE20, AH20)</f>
+        <f t="shared" si="5"/>
         <v>1.6494390000000004E-8</v>
       </c>
       <c r="F47" s="2">
@@ -16151,11 +16145,11 @@
         <v>0</v>
       </c>
       <c r="G47" s="2">
-        <f>A20</f>
+        <f t="shared" si="3"/>
         <v>4.6621999999999999E-9</v>
       </c>
       <c r="H47" s="2">
-        <f>D20</f>
+        <f t="shared" si="4"/>
         <v>1.6061E-6</v>
       </c>
     </row>
@@ -16164,19 +16158,19 @@
         <v>2.375</v>
       </c>
       <c r="B48" s="2">
-        <f>A21</f>
+        <f t="shared" si="0"/>
         <v>1.3924000000000001E-9</v>
       </c>
       <c r="C48" s="2">
-        <f>AVERAGE(D21,G21)</f>
+        <f t="shared" si="1"/>
         <v>8.7342E-7</v>
       </c>
       <c r="D48" s="2">
-        <f>AVERAGE(J22,M21,P21)</f>
+        <f t="shared" si="2"/>
         <v>4.2898666666666671E-7</v>
       </c>
       <c r="E48" s="2">
-        <f>AVERAGE(S21,V21,Y21,AB21, AE21, AH21)</f>
+        <f t="shared" si="5"/>
         <v>9.7665916666666657E-9</v>
       </c>
       <c r="F48" s="2">
@@ -16184,11 +16178,11 @@
         <v>0</v>
       </c>
       <c r="G48" s="2">
-        <f>A21</f>
+        <f t="shared" si="3"/>
         <v>1.3924000000000001E-9</v>
       </c>
       <c r="H48" s="2">
-        <f>D21</f>
+        <f t="shared" si="4"/>
         <v>6.2554000000000003E-7</v>
       </c>
     </row>
@@ -16197,19 +16191,19 @@
         <v>2.5</v>
       </c>
       <c r="B49" s="2">
-        <f>A22</f>
+        <f t="shared" si="0"/>
         <v>-2.5615999999999999E-8</v>
       </c>
       <c r="C49" s="2">
-        <f>AVERAGE(D22,G22)</f>
+        <f t="shared" si="1"/>
         <v>2.0532500000000002E-7</v>
       </c>
       <c r="D49" s="2">
-        <f>AVERAGE(J23,M22,P22)</f>
+        <f t="shared" si="2"/>
         <v>1.6227700000000002E-7</v>
       </c>
       <c r="E49" s="2">
-        <f>AVERAGE(S22,V22,Y22,AB22, AE22, AH22)</f>
+        <f t="shared" si="5"/>
         <v>2.997815E-9</v>
       </c>
       <c r="F49" s="2">
@@ -16217,11 +16211,11 @@
         <v>0</v>
       </c>
       <c r="G49" s="2">
-        <f>A22</f>
+        <f t="shared" si="3"/>
         <v>-2.5615999999999999E-8</v>
       </c>
       <c r="H49" s="2">
-        <f>D22</f>
+        <f t="shared" si="4"/>
         <v>1.0497000000000001E-7</v>
       </c>
     </row>
@@ -16230,19 +16224,19 @@
         <v>2.625</v>
       </c>
       <c r="B50" s="2">
-        <f>A23</f>
+        <f t="shared" si="0"/>
         <v>-3.6879000000000001E-9</v>
       </c>
       <c r="C50" s="2">
-        <f>AVERAGE(D23,G23)</f>
+        <f t="shared" si="1"/>
         <v>7.8678999999999999E-8</v>
       </c>
       <c r="D50" s="2">
-        <f>AVERAGE(J24,M23,P23)</f>
+        <f t="shared" si="2"/>
         <v>6.0307666666666657E-8</v>
       </c>
       <c r="E50" s="2">
-        <f>AVERAGE(S23,V23,Y23,AB23, AE23, AH23)</f>
+        <f t="shared" si="5"/>
         <v>-2.2234666666666667E-10</v>
       </c>
       <c r="F50" s="2">
@@ -16250,11 +16244,11 @@
         <v>0</v>
       </c>
       <c r="G50" s="2">
-        <f>A23</f>
+        <f t="shared" si="3"/>
         <v>-3.6879000000000001E-9</v>
       </c>
       <c r="H50" s="2">
-        <f>D23</f>
+        <f t="shared" si="4"/>
         <v>5.6897999999999998E-8</v>
       </c>
     </row>
@@ -16263,19 +16257,19 @@
         <v>2.75</v>
       </c>
       <c r="B51" s="2">
-        <f>A24</f>
+        <f t="shared" si="0"/>
         <v>-1.4001E-9</v>
       </c>
       <c r="C51" s="2">
-        <f>AVERAGE(D24,G24)</f>
+        <f t="shared" si="1"/>
         <v>2.5303000000000002E-8</v>
       </c>
       <c r="D51" s="2">
-        <f>AVERAGE(J25,M24,P24)</f>
+        <f t="shared" si="2"/>
         <v>1.5703166666666666E-8</v>
       </c>
       <c r="E51" s="2">
-        <f>AVERAGE(S24,V24,Y24,AB24, AE24, AH24)</f>
+        <f t="shared" si="5"/>
         <v>5.8023333333333316E-11</v>
       </c>
       <c r="F51" s="2">
@@ -16283,11 +16277,11 @@
         <v>0</v>
       </c>
       <c r="G51" s="2">
-        <f>A24</f>
+        <f t="shared" si="3"/>
         <v>-1.4001E-9</v>
       </c>
       <c r="H51" s="2">
-        <f>D24</f>
+        <f t="shared" si="4"/>
         <v>1.9037E-8</v>
       </c>
     </row>
@@ -16296,19 +16290,19 @@
         <v>2.875</v>
       </c>
       <c r="B52" s="2">
-        <f>A25</f>
+        <f t="shared" si="0"/>
         <v>-1.0524E-9</v>
       </c>
       <c r="C52" s="2">
-        <f>AVERAGE(D25,G25)</f>
+        <f t="shared" si="1"/>
         <v>-8.5002500000000003E-9</v>
       </c>
       <c r="D52" s="2">
-        <f>AVERAGE(J26,M25,P25)</f>
+        <f t="shared" si="2"/>
         <v>2.9761666666666664E-9</v>
       </c>
       <c r="E52" s="2">
-        <f>AVERAGE(S25,V25,Y25,AB25, AE25, AH25)</f>
+        <f t="shared" si="5"/>
         <v>3.9389299999999989E-10</v>
       </c>
       <c r="F52" s="2">
@@ -16316,11 +16310,11 @@
         <v>0</v>
       </c>
       <c r="G52" s="2">
-        <f>A25</f>
+        <f t="shared" si="3"/>
         <v>-1.0524E-9</v>
       </c>
       <c r="H52" s="2">
-        <f>D25</f>
+        <f t="shared" si="4"/>
         <v>-1.9915E-9</v>
       </c>
     </row>
@@ -16329,19 +16323,19 @@
         <v>3</v>
       </c>
       <c r="B53" s="2">
-        <f>A26</f>
+        <f t="shared" si="0"/>
         <v>-5.8027999999999999E-10</v>
       </c>
       <c r="C53" s="2">
-        <f>AVERAGE(D26,G26)</f>
+        <f t="shared" si="1"/>
         <v>7.6535000000000005E-10</v>
       </c>
       <c r="D53" s="2">
-        <f>AVERAGE(J27,M26,P26)</f>
+        <f t="shared" si="2"/>
         <v>9.9790499999999998E-10</v>
       </c>
       <c r="E53" s="2">
-        <f>AVERAGE(S26,V26,Y26,AB26, AE26, AH26)</f>
+        <f t="shared" si="5"/>
         <v>-8.9220833333333313E-11</v>
       </c>
       <c r="F53" s="2">
@@ -16349,11 +16343,11 @@
         <v>0</v>
       </c>
       <c r="G53" s="2">
-        <f>A26</f>
+        <f t="shared" si="3"/>
         <v>-5.8027999999999999E-10</v>
       </c>
       <c r="H53" s="2">
-        <f>D26</f>
+        <f t="shared" si="4"/>
         <v>2.7993E-9</v>
       </c>
     </row>
@@ -17050,8 +17044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI80"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A55" sqref="A55"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -19130,19 +19124,19 @@
         <v>0.125</v>
       </c>
       <c r="B30" s="2">
-        <f>A3</f>
+        <f t="shared" ref="B30:B53" si="0">A3</f>
         <v>-6.7791999999999997E-11</v>
       </c>
       <c r="C30" s="2">
-        <f>AVERAGE(D3,G3)</f>
+        <f t="shared" ref="C30:C53" si="1">AVERAGE(D3,G3)</f>
         <v>7.021499999999999E-10</v>
       </c>
       <c r="D30" s="2">
-        <f>AVERAGE(J4,M3,P3)</f>
+        <f t="shared" ref="D30:D53" si="2">AVERAGE(J4,M3,P3)</f>
         <v>-6.6408999999999993E-10</v>
       </c>
       <c r="E30" s="2">
-        <f>AVERAGE(S3,V3,Y3,AB3, AE3, AH3)</f>
+        <f t="shared" ref="E30:E53" si="3">AVERAGE(S3,V3,Y3,AB3, AE3, AH3)</f>
         <v>-8.6064166666666666E-11</v>
       </c>
       <c r="F30" s="2">
@@ -19150,11 +19144,11 @@
         <v>0</v>
       </c>
       <c r="G30" s="2">
-        <f>A3</f>
+        <f t="shared" ref="G30:G53" si="4">A3</f>
         <v>-6.7791999999999997E-11</v>
       </c>
       <c r="H30" s="2">
-        <f>D3</f>
+        <f t="shared" ref="H30:H53" si="5">D3</f>
         <v>2.7972999999999998E-9</v>
       </c>
     </row>
@@ -19163,19 +19157,19 @@
         <v>0.25</v>
       </c>
       <c r="B31" s="2">
-        <f>A4</f>
+        <f t="shared" si="0"/>
         <v>2.5708999999999999E-9</v>
       </c>
       <c r="C31" s="2">
-        <f>AVERAGE(D4,G4)</f>
+        <f t="shared" si="1"/>
         <v>1.044735E-8</v>
       </c>
       <c r="D31" s="2">
-        <f>AVERAGE(J5,M4,P4)</f>
+        <f t="shared" si="2"/>
         <v>1.2114333333333333E-9</v>
       </c>
       <c r="E31" s="2">
-        <f>AVERAGE(S4,V4,Y4,AB4, AE4, AH4)</f>
+        <f t="shared" si="3"/>
         <v>3.0195933333333332E-10</v>
       </c>
       <c r="F31" s="2">
@@ -19183,11 +19177,11 @@
         <v>0</v>
       </c>
       <c r="G31" s="2">
-        <f>A4</f>
+        <f t="shared" si="4"/>
         <v>2.5708999999999999E-9</v>
       </c>
       <c r="H31" s="2">
-        <f>D4</f>
+        <f t="shared" si="5"/>
         <v>4.9056999999999997E-9</v>
       </c>
     </row>
@@ -19196,19 +19190,19 @@
         <v>0.375</v>
       </c>
       <c r="B32" s="2">
-        <f>A5</f>
+        <f t="shared" si="0"/>
         <v>1.1653000000000001E-9</v>
       </c>
       <c r="C32" s="2">
-        <f>AVERAGE(D5,G5)</f>
+        <f t="shared" si="1"/>
         <v>-1.415E-9</v>
       </c>
       <c r="D32" s="2">
-        <f>AVERAGE(J6,M5,P5)</f>
+        <f t="shared" si="2"/>
         <v>1.2775233333333336E-8</v>
       </c>
       <c r="E32" s="2">
-        <f>AVERAGE(S5,V5,Y5,AB5, AE5, AH5)</f>
+        <f t="shared" si="3"/>
         <v>9.5398499999999978E-10</v>
       </c>
       <c r="F32" s="2">
@@ -19216,11 +19210,11 @@
         <v>0</v>
       </c>
       <c r="G32" s="2">
-        <f>A5</f>
+        <f t="shared" si="4"/>
         <v>1.1653000000000001E-9</v>
       </c>
       <c r="H32" s="2">
-        <f>D5</f>
+        <f t="shared" si="5"/>
         <v>2.6558999999999999E-9</v>
       </c>
     </row>
@@ -19229,19 +19223,19 @@
         <v>0.5</v>
       </c>
       <c r="B33" s="2">
-        <f>A6</f>
+        <f t="shared" si="0"/>
         <v>1.1213E-9</v>
       </c>
       <c r="C33" s="2">
-        <f>AVERAGE(D6,G6)</f>
+        <f t="shared" si="1"/>
         <v>5.6931499999999991E-9</v>
       </c>
       <c r="D33" s="2">
-        <f>AVERAGE(J7,M6,P6)</f>
+        <f t="shared" si="2"/>
         <v>-4.3353666666666668E-9</v>
       </c>
       <c r="E33" s="2">
-        <f>AVERAGE(S6,V6,Y6,AB6, AE6, AH6)</f>
+        <f t="shared" si="3"/>
         <v>1.9602499999999997E-9</v>
       </c>
       <c r="F33" s="2">
@@ -19249,11 +19243,11 @@
         <v>0</v>
       </c>
       <c r="G33" s="2">
-        <f>A6</f>
+        <f t="shared" si="4"/>
         <v>1.1213E-9</v>
       </c>
       <c r="H33" s="2">
-        <f>D6</f>
+        <f t="shared" si="5"/>
         <v>1.9980999999999999E-8</v>
       </c>
     </row>
@@ -19262,19 +19256,19 @@
         <v>0.625</v>
       </c>
       <c r="B34" s="2">
-        <f>A7</f>
+        <f t="shared" si="0"/>
         <v>-4.4657000000000001E-8</v>
       </c>
       <c r="C34" s="2">
-        <f>AVERAGE(D7,G7)</f>
+        <f t="shared" si="1"/>
         <v>5.3347999999999996E-8</v>
       </c>
       <c r="D34" s="2">
-        <f>AVERAGE(J8,M7,P7)</f>
+        <f t="shared" si="2"/>
         <v>-5.3369666666666665E-8</v>
       </c>
       <c r="E34" s="2">
-        <f>AVERAGE(S7,V7,Y7,AB7, AE7, AH7)</f>
+        <f t="shared" si="3"/>
         <v>2.3827868333333331E-9</v>
       </c>
       <c r="F34" s="2">
@@ -19282,11 +19276,11 @@
         <v>0</v>
       </c>
       <c r="G34" s="2">
-        <f>A7</f>
+        <f t="shared" si="4"/>
         <v>-4.4657000000000001E-8</v>
       </c>
       <c r="H34" s="2">
-        <f>D7</f>
+        <f t="shared" si="5"/>
         <v>9.0253999999999995E-8</v>
       </c>
     </row>
@@ -19295,19 +19289,19 @@
         <v>0.75</v>
       </c>
       <c r="B35" s="2">
-        <f>A8</f>
+        <f t="shared" si="0"/>
         <v>-2.8547000000000001E-8</v>
       </c>
       <c r="C35" s="2">
-        <f>AVERAGE(D8,G8)</f>
+        <f t="shared" si="1"/>
         <v>-1.9727000000000002E-7</v>
       </c>
       <c r="D35" s="2">
-        <f>AVERAGE(J9,M8,P8)</f>
+        <f t="shared" si="2"/>
         <v>-3.3641766666666665E-7</v>
       </c>
       <c r="E35" s="2">
-        <f>AVERAGE(S8,V8,Y8,AB8, AE8, AH8)</f>
+        <f t="shared" si="3"/>
         <v>8.7978916666666684E-9</v>
       </c>
       <c r="F35" s="2">
@@ -19315,11 +19309,11 @@
         <v>0</v>
       </c>
       <c r="G35" s="2">
-        <f>A8</f>
+        <f t="shared" si="4"/>
         <v>-2.8547000000000001E-8</v>
       </c>
       <c r="H35" s="2">
-        <f>D8</f>
+        <f t="shared" si="5"/>
         <v>-1.7814000000000001E-7</v>
       </c>
     </row>
@@ -19328,19 +19322,19 @@
         <v>0.875</v>
       </c>
       <c r="B36" s="2">
-        <f>A9</f>
+        <f t="shared" si="0"/>
         <v>-8.6357999999999998E-8</v>
       </c>
       <c r="C36" s="2">
-        <f>AVERAGE(D9,G9)</f>
+        <f t="shared" si="1"/>
         <v>-8.20875E-7</v>
       </c>
       <c r="D36" s="2">
-        <f>AVERAGE(J10,M9,P9)</f>
+        <f t="shared" si="2"/>
         <v>-1.0069826666666667E-6</v>
       </c>
       <c r="E36" s="2">
-        <f>AVERAGE(S9,V9,Y9,AB9, AE9, AH9)</f>
+        <f t="shared" si="3"/>
         <v>2.5589573333333331E-8</v>
       </c>
       <c r="F36" s="2">
@@ -19348,11 +19342,11 @@
         <v>0</v>
       </c>
       <c r="G36" s="2">
-        <f>A9</f>
+        <f t="shared" si="4"/>
         <v>-8.6357999999999998E-8</v>
       </c>
       <c r="H36" s="2">
-        <f>D9</f>
+        <f t="shared" si="5"/>
         <v>-4.7315000000000002E-7</v>
       </c>
     </row>
@@ -19361,19 +19355,19 @@
         <v>1</v>
       </c>
       <c r="B37" s="2">
-        <f>A10</f>
+        <f t="shared" si="0"/>
         <v>-4.1661999999999998E-7</v>
       </c>
       <c r="C37" s="2">
-        <f>AVERAGE(D10,G10)</f>
+        <f t="shared" si="1"/>
         <v>-2.4773E-6</v>
       </c>
       <c r="D37" s="2">
-        <f>AVERAGE(J11,M10,P10)</f>
+        <f t="shared" si="2"/>
         <v>-2.3185999999999997E-6</v>
       </c>
       <c r="E37" s="2">
-        <f>AVERAGE(S10,V10,Y10,AB10, AE10, AH10)</f>
+        <f t="shared" si="3"/>
         <v>1.4408775000000003E-8</v>
       </c>
       <c r="F37" s="2">
@@ -19381,11 +19375,11 @@
         <v>0</v>
       </c>
       <c r="G37" s="2">
-        <f>A10</f>
+        <f t="shared" si="4"/>
         <v>-4.1661999999999998E-7</v>
       </c>
       <c r="H37" s="2">
-        <f>D10</f>
+        <f t="shared" si="5"/>
         <v>-1.7935000000000001E-6</v>
       </c>
     </row>
@@ -19394,19 +19388,19 @@
         <v>1.125</v>
       </c>
       <c r="B38" s="2">
-        <f>A11</f>
+        <f t="shared" si="0"/>
         <v>-1.2598E-6</v>
       </c>
       <c r="C38" s="2">
-        <f>AVERAGE(D11,G11)</f>
+        <f t="shared" si="1"/>
         <v>-5.4543499999999997E-6</v>
       </c>
       <c r="D38" s="2">
-        <f>AVERAGE(J12,M11,P11)</f>
+        <f t="shared" si="2"/>
         <v>-3.9078666666666661E-6</v>
       </c>
       <c r="E38" s="2">
-        <f>AVERAGE(S11,V11,Y11,AB11, AE11, AH11)</f>
+        <f t="shared" si="3"/>
         <v>2.4823666666666659E-9</v>
       </c>
       <c r="F38" s="2">
@@ -19414,11 +19408,11 @@
         <v>0</v>
       </c>
       <c r="G38" s="2">
-        <f>A11</f>
+        <f t="shared" si="4"/>
         <v>-1.2598E-6</v>
       </c>
       <c r="H38" s="2">
-        <f>D11</f>
+        <f t="shared" si="5"/>
         <v>-4.2085999999999998E-6</v>
       </c>
     </row>
@@ -19427,19 +19421,19 @@
         <v>1.25</v>
       </c>
       <c r="B39" s="2">
-        <f>A12</f>
+        <f t="shared" si="0"/>
         <v>-2.0242999999999998E-6</v>
       </c>
       <c r="C39" s="2">
-        <f>AVERAGE(D12,G12)</f>
+        <f t="shared" si="1"/>
         <v>-9.4478499999999997E-6</v>
       </c>
       <c r="D39" s="2">
-        <f>AVERAGE(J13,M12,P12)</f>
+        <f t="shared" si="2"/>
         <v>-5.5649666666666658E-6</v>
       </c>
       <c r="E39" s="2">
-        <f>AVERAGE(S12,V12,Y12,AB12, AE12, AH12)</f>
+        <f t="shared" si="3"/>
         <v>2.9043949999999999E-8</v>
       </c>
       <c r="F39" s="2">
@@ -19447,11 +19441,11 @@
         <v>0</v>
       </c>
       <c r="G39" s="2">
-        <f>A12</f>
+        <f t="shared" si="4"/>
         <v>-2.0242999999999998E-6</v>
       </c>
       <c r="H39" s="2">
-        <f>D12</f>
+        <f t="shared" si="5"/>
         <v>-8.1406999999999998E-6</v>
       </c>
     </row>
@@ -19460,19 +19454,19 @@
         <v>1.375</v>
       </c>
       <c r="B40" s="2">
-        <f>A13</f>
+        <f t="shared" si="0"/>
         <v>-3.6459999999999999E-6</v>
       </c>
       <c r="C40" s="2">
-        <f>AVERAGE(D13,G13)</f>
+        <f t="shared" si="1"/>
         <v>-1.25285E-5</v>
       </c>
       <c r="D40" s="2">
-        <f>AVERAGE(J14,M13,P13)</f>
+        <f t="shared" si="2"/>
         <v>-6.8696333333333328E-6</v>
       </c>
       <c r="E40" s="2">
-        <f>AVERAGE(S13,V13,Y13,AB13, AE13, AH13)</f>
+        <f t="shared" si="3"/>
         <v>1.2011999999999981E-9</v>
       </c>
       <c r="F40" s="2">
@@ -19480,11 +19474,11 @@
         <v>0</v>
       </c>
       <c r="G40" s="2">
-        <f>A13</f>
+        <f t="shared" si="4"/>
         <v>-3.6459999999999999E-6</v>
       </c>
       <c r="H40" s="2">
-        <f>D13</f>
+        <f t="shared" si="5"/>
         <v>-1.0893999999999999E-5</v>
       </c>
     </row>
@@ -19493,19 +19487,19 @@
         <v>1.5</v>
       </c>
       <c r="B41" s="2">
-        <f>A14</f>
+        <f t="shared" si="0"/>
         <v>-5.1352999999999998E-6</v>
       </c>
       <c r="C41" s="2">
-        <f>AVERAGE(D14,G14)</f>
+        <f t="shared" si="1"/>
         <v>-1.5254499999999999E-5</v>
       </c>
       <c r="D41" s="2">
-        <f>AVERAGE(J15,M14,P14)</f>
+        <f t="shared" si="2"/>
         <v>-7.4311333333333333E-6</v>
       </c>
       <c r="E41" s="2">
-        <f>AVERAGE(S14,V14,Y14,AB14, AE14, AH14)</f>
+        <f t="shared" si="3"/>
         <v>-5.4846416666666665E-8</v>
       </c>
       <c r="F41" s="2">
@@ -19513,11 +19507,11 @@
         <v>0</v>
       </c>
       <c r="G41" s="2">
-        <f>A14</f>
+        <f t="shared" si="4"/>
         <v>-5.1352999999999998E-6</v>
       </c>
       <c r="H41" s="2">
-        <f>D14</f>
+        <f t="shared" si="5"/>
         <v>-1.3879999999999999E-5</v>
       </c>
     </row>
@@ -19526,19 +19520,19 @@
         <v>1.625</v>
       </c>
       <c r="B42" s="2">
-        <f>A15</f>
+        <f t="shared" si="0"/>
         <v>-5.2857000000000001E-6</v>
       </c>
       <c r="C42" s="2">
-        <f>AVERAGE(D15,G15)</f>
+        <f t="shared" si="1"/>
         <v>-1.65305E-5</v>
       </c>
       <c r="D42" s="2">
-        <f>AVERAGE(J16,M15,P15)</f>
+        <f t="shared" si="2"/>
         <v>-7.4338666666666667E-6</v>
       </c>
       <c r="E42" s="2">
-        <f>AVERAGE(S15,V15,Y15,AB15, AE15, AH15)</f>
+        <f t="shared" si="3"/>
         <v>-5.495376666666666E-8</v>
       </c>
       <c r="F42" s="2">
@@ -19546,11 +19540,11 @@
         <v>0</v>
       </c>
       <c r="G42" s="2">
-        <f>A15</f>
+        <f t="shared" si="4"/>
         <v>-5.2857000000000001E-6</v>
       </c>
       <c r="H42" s="2">
-        <f>D15</f>
+        <f t="shared" si="5"/>
         <v>-1.5234E-5</v>
       </c>
     </row>
@@ -19559,19 +19553,19 @@
         <v>1.75</v>
       </c>
       <c r="B43" s="2">
-        <f>A16</f>
+        <f t="shared" si="0"/>
         <v>-4.8449E-6</v>
       </c>
       <c r="C43" s="2">
-        <f>AVERAGE(D16,G16)</f>
+        <f t="shared" si="1"/>
         <v>-1.5425000000000002E-5</v>
       </c>
       <c r="D43" s="2">
-        <f>AVERAGE(J17,M16,P16)</f>
+        <f t="shared" si="2"/>
         <v>-6.5820999999999992E-6</v>
       </c>
       <c r="E43" s="2">
-        <f>AVERAGE(S16,V16,Y16,AB16, AE16, AH16)</f>
+        <f t="shared" si="3"/>
         <v>-1.1103700000000002E-8</v>
       </c>
       <c r="F43" s="2">
@@ -19579,11 +19573,11 @@
         <v>0</v>
       </c>
       <c r="G43" s="2">
-        <f>A16</f>
+        <f t="shared" si="4"/>
         <v>-4.8449E-6</v>
       </c>
       <c r="H43" s="2">
-        <f>D16</f>
+        <f t="shared" si="5"/>
         <v>-1.4321999999999999E-5</v>
       </c>
     </row>
@@ -19592,19 +19586,19 @@
         <v>1.875</v>
       </c>
       <c r="B44" s="2">
-        <f>A17</f>
+        <f t="shared" si="0"/>
         <v>-3.7266E-6</v>
       </c>
       <c r="C44" s="2">
-        <f>AVERAGE(D17,G17)</f>
+        <f t="shared" si="1"/>
         <v>-1.2805999999999999E-5</v>
       </c>
       <c r="D44" s="2">
-        <f>AVERAGE(J18,M17,P17)</f>
+        <f t="shared" si="2"/>
         <v>-5.6851333333333334E-6</v>
       </c>
       <c r="E44" s="2">
-        <f>AVERAGE(S17,V17,Y17,AB17, AE17, AH17)</f>
+        <f t="shared" si="3"/>
         <v>-2.1374099999999999E-8</v>
       </c>
       <c r="F44" s="2">
@@ -19612,11 +19606,11 @@
         <v>0</v>
       </c>
       <c r="G44" s="2">
-        <f>A17</f>
+        <f t="shared" si="4"/>
         <v>-3.7266E-6</v>
       </c>
       <c r="H44" s="2">
-        <f>D17</f>
+        <f t="shared" si="5"/>
         <v>-1.1917E-5</v>
       </c>
     </row>
@@ -19625,19 +19619,19 @@
         <v>2</v>
       </c>
       <c r="B45" s="2">
-        <f>A18</f>
+        <f t="shared" si="0"/>
         <v>-2.3049000000000002E-6</v>
       </c>
       <c r="C45" s="2">
-        <f>AVERAGE(D18,G18)</f>
+        <f t="shared" si="1"/>
         <v>-9.3859000000000011E-6</v>
       </c>
       <c r="D45" s="2">
-        <f>AVERAGE(J19,M18,P18)</f>
+        <f t="shared" si="2"/>
         <v>-3.8707000000000001E-6</v>
       </c>
       <c r="E45" s="2">
-        <f>AVERAGE(S18,V18,Y18,AB18, AE18, AH18)</f>
+        <f t="shared" si="3"/>
         <v>1.265208333333333E-8</v>
       </c>
       <c r="F45" s="2">
@@ -19645,11 +19639,11 @@
         <v>0</v>
       </c>
       <c r="G45" s="2">
-        <f>A18</f>
+        <f t="shared" si="4"/>
         <v>-2.3049000000000002E-6</v>
       </c>
       <c r="H45" s="2">
-        <f>D18</f>
+        <f t="shared" si="5"/>
         <v>-7.8547999999999997E-6</v>
       </c>
     </row>
@@ -19658,19 +19652,19 @@
         <v>2.125</v>
       </c>
       <c r="B46" s="2">
-        <f>A19</f>
+        <f t="shared" si="0"/>
         <v>-9.9627999999999997E-7</v>
       </c>
       <c r="C46" s="2">
-        <f>AVERAGE(D19,G19)</f>
+        <f t="shared" si="1"/>
         <v>-5.73105E-6</v>
       </c>
       <c r="D46" s="2">
-        <f>AVERAGE(J20,M19,P19)</f>
+        <f t="shared" si="2"/>
         <v>-2.2125833333333331E-6</v>
       </c>
       <c r="E46" s="2">
-        <f>AVERAGE(S19,V19,Y19,AB19, AE19, AH19)</f>
+        <f t="shared" si="3"/>
         <v>1.8271583333333335E-9</v>
       </c>
       <c r="F46" s="2">
@@ -19678,11 +19672,11 @@
         <v>0</v>
       </c>
       <c r="G46" s="2">
-        <f>A19</f>
+        <f t="shared" si="4"/>
         <v>-9.9627999999999997E-7</v>
       </c>
       <c r="H46" s="2">
-        <f>D19</f>
+        <f t="shared" si="5"/>
         <v>-4.7207000000000004E-6</v>
       </c>
     </row>
@@ -19691,19 +19685,19 @@
         <v>2.25</v>
       </c>
       <c r="B47" s="2">
-        <f>A20</f>
+        <f t="shared" si="0"/>
         <v>-5.7164999999999996E-7</v>
       </c>
       <c r="C47" s="2">
-        <f>AVERAGE(D20,G20)</f>
+        <f t="shared" si="1"/>
         <v>-2.93335E-6</v>
       </c>
       <c r="D47" s="2">
-        <f>AVERAGE(J21,M20,P20)</f>
+        <f t="shared" si="2"/>
         <v>-1.0276133333333334E-6</v>
       </c>
       <c r="E47" s="2">
-        <f>AVERAGE(S20,V20,Y20,AB20, AE20, AH20)</f>
+        <f t="shared" si="3"/>
         <v>3.7733333333333334E-8</v>
       </c>
       <c r="F47" s="2">
@@ -19711,11 +19705,11 @@
         <v>0</v>
       </c>
       <c r="G47" s="2">
-        <f>A20</f>
+        <f t="shared" si="4"/>
         <v>-5.7164999999999996E-7</v>
       </c>
       <c r="H47" s="2">
-        <f>D20</f>
+        <f t="shared" si="5"/>
         <v>-2.2307999999999999E-6</v>
       </c>
     </row>
@@ -19724,19 +19718,19 @@
         <v>2.375</v>
       </c>
       <c r="B48" s="2">
-        <f>A21</f>
+        <f t="shared" si="0"/>
         <v>-1.808E-7</v>
       </c>
       <c r="C48" s="2">
-        <f>AVERAGE(D21,G21)</f>
+        <f t="shared" si="1"/>
         <v>-9.5808000000000007E-7</v>
       </c>
       <c r="D48" s="2">
-        <f>AVERAGE(J22,M21,P21)</f>
+        <f t="shared" si="2"/>
         <v>-2.4560599999999998E-7</v>
       </c>
       <c r="E48" s="2">
-        <f>AVERAGE(S21,V21,Y21,AB21, AE21, AH21)</f>
+        <f t="shared" si="3"/>
         <v>2.4291888333333336E-8</v>
       </c>
       <c r="F48" s="2">
@@ -19744,11 +19738,11 @@
         <v>0</v>
       </c>
       <c r="G48" s="2">
-        <f>A21</f>
+        <f t="shared" si="4"/>
         <v>-1.808E-7</v>
       </c>
       <c r="H48" s="2">
-        <f>D21</f>
+        <f t="shared" si="5"/>
         <v>-5.7456000000000003E-7</v>
       </c>
     </row>
@@ -19757,19 +19751,19 @@
         <v>2.5</v>
       </c>
       <c r="B49" s="2">
-        <f>A22</f>
+        <f t="shared" si="0"/>
         <v>-4.0337999999999999E-9</v>
       </c>
       <c r="C49" s="2">
-        <f>AVERAGE(D22,G22)</f>
+        <f t="shared" si="1"/>
         <v>-2.3488500000000003E-7</v>
       </c>
       <c r="D49" s="2">
-        <f>AVERAGE(J23,M22,P22)</f>
+        <f t="shared" si="2"/>
         <v>-5.8004666666666673E-8</v>
       </c>
       <c r="E49" s="2">
-        <f>AVERAGE(S22,V22,Y22,AB22, AE22, AH22)</f>
+        <f t="shared" si="3"/>
         <v>7.7201816666666668E-9</v>
       </c>
       <c r="F49" s="2">
@@ -19777,11 +19771,11 @@
         <v>0</v>
       </c>
       <c r="G49" s="2">
-        <f>A22</f>
+        <f t="shared" si="4"/>
         <v>-4.0337999999999999E-9</v>
       </c>
       <c r="H49" s="2">
-        <f>D22</f>
+        <f t="shared" si="5"/>
         <v>-1.2917000000000001E-7</v>
       </c>
     </row>
@@ -19790,19 +19784,19 @@
         <v>2.625</v>
       </c>
       <c r="B50" s="2">
-        <f>A23</f>
+        <f t="shared" si="0"/>
         <v>2.8487999999999999E-9</v>
       </c>
       <c r="C50" s="2">
-        <f>AVERAGE(D23,G23)</f>
+        <f t="shared" si="1"/>
         <v>-3.8819499999999999E-8</v>
       </c>
       <c r="D50" s="2">
-        <f>AVERAGE(J24,M23,P23)</f>
+        <f t="shared" si="2"/>
         <v>2.0965666666666665E-8</v>
       </c>
       <c r="E50" s="2">
-        <f>AVERAGE(S23,V23,Y23,AB23, AE23, AH23)</f>
+        <f t="shared" si="3"/>
         <v>2.1817199999999998E-9</v>
       </c>
       <c r="F50" s="2">
@@ -19810,11 +19804,11 @@
         <v>0</v>
       </c>
       <c r="G50" s="2">
-        <f>A23</f>
+        <f t="shared" si="4"/>
         <v>2.8487999999999999E-9</v>
       </c>
       <c r="H50" s="2">
-        <f>D23</f>
+        <f t="shared" si="5"/>
         <v>-3.2923999999999998E-8</v>
       </c>
     </row>
@@ -19823,19 +19817,19 @@
         <v>2.75</v>
       </c>
       <c r="B51" s="2">
-        <f>A24</f>
+        <f t="shared" si="0"/>
         <v>-2.969E-9</v>
       </c>
       <c r="C51" s="2">
-        <f>AVERAGE(D24,G24)</f>
+        <f t="shared" si="1"/>
         <v>2.557332E-8</v>
       </c>
       <c r="D51" s="2">
-        <f>AVERAGE(J25,M24,P24)</f>
+        <f t="shared" si="2"/>
         <v>6.2434333333333331E-9</v>
       </c>
       <c r="E51" s="2">
-        <f>AVERAGE(S24,V24,Y24,AB24, AE24, AH24)</f>
+        <f t="shared" si="3"/>
         <v>8.6966500000000002E-10</v>
       </c>
       <c r="F51" s="2">
@@ -19843,11 +19837,11 @@
         <v>0</v>
       </c>
       <c r="G51" s="2">
-        <f>A24</f>
+        <f t="shared" si="4"/>
         <v>-2.969E-9</v>
       </c>
       <c r="H51" s="2">
-        <f>D24</f>
+        <f t="shared" si="5"/>
         <v>-1.1935999999999999E-10</v>
       </c>
     </row>
@@ -19856,19 +19850,19 @@
         <v>2.875</v>
       </c>
       <c r="B52" s="2">
-        <f>A25</f>
+        <f t="shared" si="0"/>
         <v>-5.2440999999999995E-10</v>
       </c>
       <c r="C52" s="2">
-        <f>AVERAGE(D25,G25)</f>
+        <f t="shared" si="1"/>
         <v>1.5584700000000001E-8</v>
       </c>
       <c r="D52" s="2">
-        <f>AVERAGE(J26,M25,P25)</f>
+        <f t="shared" si="2"/>
         <v>8.9595666666666674E-9</v>
       </c>
       <c r="E52" s="2">
-        <f>AVERAGE(S25,V25,Y25,AB25, AE25, AH25)</f>
+        <f t="shared" si="3"/>
         <v>-3.1706100000000005E-10</v>
       </c>
       <c r="F52" s="2">
@@ -19876,11 +19870,11 @@
         <v>0</v>
       </c>
       <c r="G52" s="2">
-        <f>A25</f>
+        <f t="shared" si="4"/>
         <v>-5.2440999999999995E-10</v>
       </c>
       <c r="H52" s="2">
-        <f>D25</f>
+        <f t="shared" si="5"/>
         <v>2.5416000000000001E-8</v>
       </c>
     </row>
@@ -19889,19 +19883,19 @@
         <v>3</v>
       </c>
       <c r="B53" s="2">
-        <f>A26</f>
+        <f t="shared" si="0"/>
         <v>-7.6054999999999998E-9</v>
       </c>
       <c r="C53" s="2">
-        <f>AVERAGE(D26,G26)</f>
+        <f t="shared" si="1"/>
         <v>-6.8739999999999992E-10</v>
       </c>
       <c r="D53" s="2">
-        <f>AVERAGE(J27,M26,P26)</f>
+        <f t="shared" si="2"/>
         <v>3.5875999999999999E-9</v>
       </c>
       <c r="E53" s="2">
-        <f>AVERAGE(S26,V26,Y26,AB26, AE26, AH26)</f>
+        <f t="shared" si="3"/>
         <v>1.817891666666666E-10</v>
       </c>
       <c r="F53" s="2">
@@ -19909,11 +19903,11 @@
         <v>0</v>
       </c>
       <c r="G53" s="2">
-        <f>A26</f>
+        <f t="shared" si="4"/>
         <v>-7.6054999999999998E-9</v>
       </c>
       <c r="H53" s="2">
-        <f>D26</f>
+        <f t="shared" si="5"/>
         <v>7.4326999999999998E-9</v>
       </c>
     </row>
@@ -20610,8 +20604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AI109"/>
   <sheetViews>
-    <sheetView topLeftCell="A59" workbookViewId="0">
-      <selection activeCell="A85" sqref="A85:H109"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23470,31 +23464,31 @@
         <v>0.125</v>
       </c>
       <c r="B58" s="2">
-        <f>-A30</f>
+        <f t="shared" ref="B58:H67" si="6">-A30</f>
         <v>-1.3604E-9</v>
       </c>
       <c r="C58" s="2">
-        <f>-B30</f>
+        <f t="shared" si="6"/>
         <v>-6.65355E-9</v>
       </c>
       <c r="D58" s="2">
-        <f>-C30</f>
+        <f t="shared" si="6"/>
         <v>-1.978996666666667E-9</v>
       </c>
       <c r="E58" s="2">
-        <f>-D30</f>
+        <f t="shared" si="6"/>
         <v>-1.1304831499999999E-10</v>
       </c>
       <c r="F58" s="2">
-        <f>-E30</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G58" s="2">
-        <f>-F30</f>
+        <f t="shared" si="6"/>
         <v>-1.3604E-9</v>
       </c>
       <c r="H58" s="2">
-        <f>-G30</f>
+        <f t="shared" si="6"/>
         <v>-1.9600999999999999E-9</v>
       </c>
     </row>
@@ -23503,31 +23497,31 @@
         <v>0.25</v>
       </c>
       <c r="B59" s="2">
-        <f>-A31</f>
+        <f t="shared" si="6"/>
         <v>9.8081999999999993E-10</v>
       </c>
       <c r="C59" s="2">
-        <f>-B31</f>
+        <f t="shared" si="6"/>
         <v>-1.9532499999999996E-9</v>
       </c>
       <c r="D59" s="2">
-        <f>-C31</f>
+        <f t="shared" si="6"/>
         <v>5.4178200000000006E-9</v>
       </c>
       <c r="E59" s="2">
-        <f>-D31</f>
+        <f t="shared" si="6"/>
         <v>-5.7701633333333338E-10</v>
       </c>
       <c r="F59" s="2">
-        <f>-E31</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G59" s="2">
-        <f>-F31</f>
+        <f t="shared" si="6"/>
         <v>9.8081999999999993E-10</v>
       </c>
       <c r="H59" s="2">
-        <f>-G31</f>
+        <f t="shared" si="6"/>
         <v>5.4078000000000003E-9</v>
       </c>
     </row>
@@ -23536,31 +23530,31 @@
         <v>0.375</v>
       </c>
       <c r="B60" s="2">
-        <f>-A32</f>
+        <f t="shared" si="6"/>
         <v>3.8039999999999997E-9</v>
       </c>
       <c r="C60" s="2">
-        <f>-B32</f>
+        <f t="shared" si="6"/>
         <v>1.91158E-8</v>
       </c>
       <c r="D60" s="2">
-        <f>-C32</f>
+        <f t="shared" si="6"/>
         <v>-1.0599833333333333E-8</v>
       </c>
       <c r="E60" s="2">
-        <f>-D32</f>
+        <f t="shared" si="6"/>
         <v>-9.0190316666666677E-10</v>
       </c>
       <c r="F60" s="2">
-        <f>-E32</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G60" s="2">
-        <f>-F32</f>
+        <f t="shared" si="6"/>
         <v>3.8039999999999997E-9</v>
       </c>
       <c r="H60" s="2">
-        <f>-G32</f>
+        <f t="shared" si="6"/>
         <v>3.4940000000000001E-8</v>
       </c>
     </row>
@@ -23569,31 +23563,31 @@
         <v>0.5</v>
       </c>
       <c r="B61" s="2">
-        <f>-A33</f>
+        <f t="shared" si="6"/>
         <v>3.7155999999999999E-8</v>
       </c>
       <c r="C61" s="2">
-        <f>-B33</f>
+        <f t="shared" si="6"/>
         <v>1.6717500000000001E-7</v>
       </c>
       <c r="D61" s="2">
-        <f>-C33</f>
+        <f t="shared" si="6"/>
         <v>7.7106666666666661E-8</v>
       </c>
       <c r="E61" s="2">
-        <f>-D33</f>
+        <f t="shared" si="6"/>
         <v>-3.4863166666666656E-10</v>
       </c>
       <c r="F61" s="2">
-        <f>-E33</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G61" s="2">
-        <f>-F33</f>
+        <f t="shared" si="6"/>
         <v>3.7155999999999999E-8</v>
       </c>
       <c r="H61" s="2">
-        <f>-G33</f>
+        <f t="shared" si="6"/>
         <v>1.4447E-7</v>
       </c>
     </row>
@@ -23602,31 +23596,31 @@
         <v>0.625</v>
       </c>
       <c r="B62" s="2">
-        <f>-A34</f>
+        <f t="shared" si="6"/>
         <v>2.7223000000000002E-8</v>
       </c>
       <c r="C62" s="2">
-        <f>-B34</f>
+        <f t="shared" si="6"/>
         <v>1.2924000000000001E-7</v>
       </c>
       <c r="D62" s="2">
-        <f>-C34</f>
+        <f t="shared" si="6"/>
         <v>3.5932233333333326E-7</v>
       </c>
       <c r="E62" s="2">
-        <f>-D34</f>
+        <f t="shared" si="6"/>
         <v>1.2090316666666666E-8</v>
       </c>
       <c r="F62" s="2">
-        <f>-E34</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G62" s="2">
-        <f>-F34</f>
+        <f t="shared" si="6"/>
         <v>2.7223000000000002E-8</v>
       </c>
       <c r="H62" s="2">
-        <f>-G34</f>
+        <f t="shared" si="6"/>
         <v>1.1758E-7</v>
       </c>
     </row>
@@ -23635,31 +23629,31 @@
         <v>0.75</v>
       </c>
       <c r="B63" s="2">
-        <f>-A35</f>
+        <f t="shared" si="6"/>
         <v>2.7897000000000002E-7</v>
       </c>
       <c r="C63" s="2">
-        <f>-B35</f>
+        <f t="shared" si="6"/>
         <v>1.1776500000000001E-6</v>
       </c>
       <c r="D63" s="2">
-        <f>-C35</f>
+        <f t="shared" si="6"/>
         <v>1.3048333333333334E-6</v>
       </c>
       <c r="E63" s="2">
-        <f>-D35</f>
+        <f t="shared" si="6"/>
         <v>5.3766116666666655E-9</v>
       </c>
       <c r="F63" s="2">
-        <f>-E35</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G63" s="2">
-        <f>-F35</f>
+        <f t="shared" si="6"/>
         <v>2.7897000000000002E-7</v>
       </c>
       <c r="H63" s="2">
-        <f>-G35</f>
+        <f t="shared" si="6"/>
         <v>1.1102E-6</v>
       </c>
     </row>
@@ -23668,31 +23662,31 @@
         <v>0.875</v>
       </c>
       <c r="B64" s="2">
-        <f>-A36</f>
+        <f t="shared" si="6"/>
         <v>7.8148000000000003E-7</v>
       </c>
       <c r="C64" s="2">
-        <f>-B36</f>
+        <f t="shared" si="6"/>
         <v>3.3079500000000002E-6</v>
       </c>
       <c r="D64" s="2">
-        <f>-C36</f>
+        <f t="shared" si="6"/>
         <v>3.1211866666666666E-6</v>
       </c>
       <c r="E64" s="2">
-        <f>-D36</f>
+        <f t="shared" si="6"/>
         <v>-5.9533333333333314E-10</v>
       </c>
       <c r="F64" s="2">
-        <f>-E36</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G64" s="2">
-        <f>-F36</f>
+        <f t="shared" si="6"/>
         <v>7.8148000000000003E-7</v>
       </c>
       <c r="H64" s="2">
-        <f>-G36</f>
+        <f t="shared" si="6"/>
         <v>2.9720000000000001E-6</v>
       </c>
     </row>
@@ -23701,31 +23695,31 @@
         <v>1</v>
       </c>
       <c r="B65" s="2">
-        <f>-A37</f>
+        <f t="shared" si="6"/>
         <v>2.0884000000000002E-6</v>
       </c>
       <c r="C65" s="2">
-        <f>-B37</f>
+        <f t="shared" si="6"/>
         <v>8.3693999999999999E-6</v>
       </c>
       <c r="D65" s="2">
-        <f>-C37</f>
+        <f t="shared" si="6"/>
         <v>6.262530000000001E-6</v>
       </c>
       <c r="E65" s="2">
-        <f>-D37</f>
+        <f t="shared" si="6"/>
         <v>1.3889999999999999E-8</v>
       </c>
       <c r="F65" s="2">
-        <f>-E37</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G65" s="2">
-        <f>-F37</f>
+        <f t="shared" si="6"/>
         <v>2.0884000000000002E-6</v>
       </c>
       <c r="H65" s="2">
-        <f>-G37</f>
+        <f t="shared" si="6"/>
         <v>6.8491000000000002E-6</v>
       </c>
     </row>
@@ -23734,31 +23728,31 @@
         <v>1.125</v>
       </c>
       <c r="B66" s="2">
-        <f>-A38</f>
+        <f t="shared" si="6"/>
         <v>4.6666999999999997E-6</v>
       </c>
       <c r="C66" s="2">
-        <f>-B38</f>
+        <f t="shared" si="6"/>
         <v>1.5378499999999999E-5</v>
       </c>
       <c r="D66" s="2">
-        <f>-C38</f>
+        <f t="shared" si="6"/>
         <v>1.07987E-5</v>
       </c>
       <c r="E66" s="2">
-        <f>-D38</f>
+        <f t="shared" si="6"/>
         <v>5.8905183333333338E-8</v>
       </c>
       <c r="F66" s="2">
-        <f>-E38</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G66" s="2">
-        <f>-F38</f>
+        <f t="shared" si="6"/>
         <v>4.6666999999999997E-6</v>
       </c>
       <c r="H66" s="2">
-        <f>-G38</f>
+        <f t="shared" si="6"/>
         <v>1.2223E-5</v>
       </c>
     </row>
@@ -23767,31 +23761,31 @@
         <v>1.25</v>
       </c>
       <c r="B67" s="2">
-        <f>-A39</f>
+        <f t="shared" si="6"/>
         <v>7.7236E-6</v>
       </c>
       <c r="C67" s="2">
-        <f>-B39</f>
+        <f t="shared" si="6"/>
         <v>2.4887000000000001E-5</v>
       </c>
       <c r="D67" s="2">
-        <f>-C39</f>
+        <f t="shared" si="6"/>
         <v>1.4170433333333336E-5</v>
       </c>
       <c r="E67" s="2">
-        <f>-D39</f>
+        <f t="shared" si="6"/>
         <v>1.7209266000000004E-7</v>
       </c>
       <c r="F67" s="2">
-        <f>-E39</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="G67" s="2">
-        <f>-F39</f>
+        <f t="shared" si="6"/>
         <v>7.7236E-6</v>
       </c>
       <c r="H67" s="2">
-        <f>-G39</f>
+        <f t="shared" si="6"/>
         <v>2.0801999999999998E-5</v>
       </c>
     </row>
@@ -23800,31 +23794,31 @@
         <v>1.375</v>
       </c>
       <c r="B68" s="2">
-        <f>-A40</f>
+        <f t="shared" ref="B68:H77" si="7">-A40</f>
         <v>1.2843000000000001E-5</v>
       </c>
       <c r="C68" s="2">
-        <f>-B40</f>
+        <f t="shared" si="7"/>
         <v>3.4558999999999999E-5</v>
       </c>
       <c r="D68" s="2">
-        <f>-C40</f>
+        <f t="shared" si="7"/>
         <v>1.8744466666666666E-5</v>
       </c>
       <c r="E68" s="2">
-        <f>-D40</f>
+        <f t="shared" si="7"/>
         <v>2.1209306666666667E-7</v>
       </c>
       <c r="F68" s="2">
-        <f>-E40</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G68" s="2">
-        <f>-F40</f>
+        <f t="shared" si="7"/>
         <v>1.2843000000000001E-5</v>
       </c>
       <c r="H68" s="2">
-        <f>-G40</f>
+        <f t="shared" si="7"/>
         <v>3.0954999999999998E-5</v>
       </c>
     </row>
@@ -23833,31 +23827,31 @@
         <v>1.5</v>
       </c>
       <c r="B69" s="2">
-        <f>-A41</f>
+        <f t="shared" si="7"/>
         <v>1.6935E-5</v>
       </c>
       <c r="C69" s="2">
-        <f>-B41</f>
+        <f t="shared" si="7"/>
         <v>4.0263999999999999E-5</v>
       </c>
       <c r="D69" s="2">
-        <f>-C41</f>
+        <f t="shared" si="7"/>
         <v>1.9461466666666667E-5</v>
       </c>
       <c r="E69" s="2">
-        <f>-D41</f>
+        <f t="shared" si="7"/>
         <v>3.1091849999999999E-7</v>
       </c>
       <c r="F69" s="2">
-        <f>-E41</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G69" s="2">
-        <f>-F41</f>
+        <f t="shared" si="7"/>
         <v>1.6935E-5</v>
       </c>
       <c r="H69" s="2">
-        <f>-G41</f>
+        <f t="shared" si="7"/>
         <v>3.7913000000000001E-5</v>
       </c>
     </row>
@@ -23866,31 +23860,31 @@
         <v>1.625</v>
       </c>
       <c r="B70" s="2">
-        <f>-A42</f>
+        <f t="shared" si="7"/>
         <v>1.7543000000000001E-5</v>
       </c>
       <c r="C70" s="2">
-        <f>-B42</f>
+        <f t="shared" si="7"/>
         <v>4.2313500000000001E-5</v>
       </c>
       <c r="D70" s="2">
-        <f>-C42</f>
+        <f t="shared" si="7"/>
         <v>1.9834699999999998E-5</v>
       </c>
       <c r="E70" s="2">
-        <f>-D42</f>
+        <f t="shared" si="7"/>
         <v>3.987865E-7</v>
       </c>
       <c r="F70" s="2">
-        <f>-E42</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G70" s="2">
-        <f>-F42</f>
+        <f t="shared" si="7"/>
         <v>1.7543000000000001E-5</v>
       </c>
       <c r="H70" s="2">
-        <f>-G42</f>
+        <f t="shared" si="7"/>
         <v>4.0595E-5</v>
       </c>
     </row>
@@ -23899,31 +23893,31 @@
         <v>1.75</v>
       </c>
       <c r="B71" s="2">
-        <f>-A43</f>
+        <f t="shared" si="7"/>
         <v>1.59E-5</v>
       </c>
       <c r="C71" s="2">
-        <f>-B43</f>
+        <f t="shared" si="7"/>
         <v>4.1788500000000001E-5</v>
       </c>
       <c r="D71" s="2">
-        <f>-C43</f>
+        <f t="shared" si="7"/>
         <v>1.8183699999999997E-5</v>
       </c>
       <c r="E71" s="2">
-        <f>-D43</f>
+        <f t="shared" si="7"/>
         <v>3.8535933333333327E-7</v>
       </c>
       <c r="F71" s="2">
-        <f>-E43</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G71" s="2">
-        <f>-F43</f>
+        <f t="shared" si="7"/>
         <v>1.59E-5</v>
       </c>
       <c r="H71" s="2">
-        <f>-G43</f>
+        <f t="shared" si="7"/>
         <v>4.0373000000000001E-5</v>
       </c>
     </row>
@@ -23932,31 +23926,31 @@
         <v>1.875</v>
       </c>
       <c r="B72" s="2">
-        <f>-A44</f>
+        <f t="shared" si="7"/>
         <v>1.2404E-5</v>
       </c>
       <c r="C72" s="2">
-        <f>-B44</f>
+        <f t="shared" si="7"/>
         <v>3.4632000000000003E-5</v>
       </c>
       <c r="D72" s="2">
-        <f>-C44</f>
+        <f t="shared" si="7"/>
         <v>1.4192300000000001E-5</v>
       </c>
       <c r="E72" s="2">
-        <f>-D44</f>
+        <f t="shared" si="7"/>
         <v>3.3667451666666663E-7</v>
       </c>
       <c r="F72" s="2">
-        <f>-E44</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G72" s="2">
-        <f>-F44</f>
+        <f t="shared" si="7"/>
         <v>1.2404E-5</v>
       </c>
       <c r="H72" s="2">
-        <f>-G44</f>
+        <f t="shared" si="7"/>
         <v>3.1791000000000001E-5</v>
       </c>
     </row>
@@ -23965,31 +23959,31 @@
         <v>2</v>
       </c>
       <c r="B73" s="2">
-        <f>-A45</f>
+        <f t="shared" si="7"/>
         <v>8.5442000000000003E-6</v>
       </c>
       <c r="C73" s="2">
-        <f>-B45</f>
+        <f t="shared" si="7"/>
         <v>2.5250499999999998E-5</v>
       </c>
       <c r="D73" s="2">
-        <f>-C45</f>
+        <f t="shared" si="7"/>
         <v>1.0715233333333334E-5</v>
       </c>
       <c r="E73" s="2">
-        <f>-D45</f>
+        <f t="shared" si="7"/>
         <v>1.4019916666666667E-7</v>
       </c>
       <c r="F73" s="2">
-        <f>-E45</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G73" s="2">
-        <f>-F45</f>
+        <f t="shared" si="7"/>
         <v>8.5442000000000003E-6</v>
       </c>
       <c r="H73" s="2">
-        <f>-G45</f>
+        <f t="shared" si="7"/>
         <v>2.2594000000000001E-5</v>
       </c>
     </row>
@@ -23998,31 +23992,31 @@
         <v>2.125</v>
       </c>
       <c r="B74" s="2">
-        <f>-A46</f>
+        <f t="shared" si="7"/>
         <v>4.8806999999999997E-6</v>
       </c>
       <c r="C74" s="2">
-        <f>-B46</f>
+        <f t="shared" si="7"/>
         <v>1.6206500000000001E-5</v>
       </c>
       <c r="D74" s="2">
-        <f>-C46</f>
+        <f t="shared" si="7"/>
         <v>6.2978333333333335E-6</v>
       </c>
       <c r="E74" s="2">
-        <f>-D46</f>
+        <f t="shared" si="7"/>
         <v>1.3284749999999999E-7</v>
       </c>
       <c r="F74" s="2">
-        <f>-E46</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G74" s="2">
-        <f>-F46</f>
+        <f t="shared" si="7"/>
         <v>4.8806999999999997E-6</v>
       </c>
       <c r="H74" s="2">
-        <f>-G46</f>
+        <f t="shared" si="7"/>
         <v>1.4195E-5</v>
       </c>
     </row>
@@ -24031,31 +24025,31 @@
         <v>2.25</v>
       </c>
       <c r="B75" s="2">
-        <f>-A47</f>
+        <f t="shared" si="7"/>
         <v>2.2827000000000002E-6</v>
       </c>
       <c r="C75" s="2">
-        <f>-B47</f>
+        <f t="shared" si="7"/>
         <v>8.9399500000000007E-6</v>
       </c>
       <c r="D75" s="2">
-        <f>-C47</f>
+        <f t="shared" si="7"/>
         <v>2.9341100000000003E-6</v>
       </c>
       <c r="E75" s="2">
-        <f>-D47</f>
+        <f t="shared" si="7"/>
         <v>2.9714951666666667E-8</v>
       </c>
       <c r="F75" s="2">
-        <f>-E47</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G75" s="2">
-        <f>-F47</f>
+        <f t="shared" si="7"/>
         <v>2.2827000000000002E-6</v>
       </c>
       <c r="H75" s="2">
-        <f>-G47</f>
+        <f t="shared" si="7"/>
         <v>7.4858999999999998E-6</v>
       </c>
     </row>
@@ -24064,31 +24058,31 @@
         <v>2.375</v>
       </c>
       <c r="B76" s="2">
-        <f>-A48</f>
+        <f t="shared" si="7"/>
         <v>1.2347E-6</v>
       </c>
       <c r="C76" s="2">
-        <f>-B48</f>
+        <f t="shared" si="7"/>
         <v>3.0713999999999999E-6</v>
       </c>
       <c r="D76" s="2">
-        <f>-C48</f>
+        <f t="shared" si="7"/>
         <v>8.5529099999999995E-7</v>
       </c>
       <c r="E76" s="2">
-        <f>-D48</f>
+        <f t="shared" si="7"/>
         <v>7.4866500000000021E-9</v>
       </c>
       <c r="F76" s="2">
-        <f>-E48</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G76" s="2">
-        <f>-F48</f>
+        <f t="shared" si="7"/>
         <v>1.2347E-6</v>
       </c>
       <c r="H76" s="2">
-        <f>-G48</f>
+        <f t="shared" si="7"/>
         <v>2.2925000000000001E-6</v>
       </c>
     </row>
@@ -24097,31 +24091,31 @@
         <v>2.5</v>
       </c>
       <c r="B77" s="2">
-        <f>-A49</f>
+        <f t="shared" si="7"/>
         <v>2.7469999999999999E-7</v>
       </c>
       <c r="C77" s="2">
-        <f>-B49</f>
+        <f t="shared" si="7"/>
         <v>1.0838999999999999E-6</v>
       </c>
       <c r="D77" s="2">
-        <f>-C49</f>
+        <f t="shared" si="7"/>
         <v>5.2519833333333336E-7</v>
       </c>
       <c r="E77" s="2">
-        <f>-D49</f>
+        <f t="shared" si="7"/>
         <v>1.7095004999999997E-8</v>
       </c>
       <c r="F77" s="2">
-        <f>-E49</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="G77" s="2">
-        <f>-F49</f>
+        <f t="shared" si="7"/>
         <v>2.7469999999999999E-7</v>
       </c>
       <c r="H77" s="2">
-        <f>-G49</f>
+        <f t="shared" si="7"/>
         <v>7.85E-7</v>
       </c>
     </row>
@@ -24130,31 +24124,31 @@
         <v>2.625</v>
       </c>
       <c r="B78" s="2">
-        <f>-A50</f>
+        <f t="shared" ref="B78:H87" si="8">-A50</f>
         <v>1.2386E-7</v>
       </c>
       <c r="C78" s="2">
-        <f>-B50</f>
+        <f t="shared" si="8"/>
         <v>4.14605E-7</v>
       </c>
       <c r="D78" s="2">
-        <f>-C50</f>
+        <f t="shared" si="8"/>
         <v>2.1936333333333335E-8</v>
       </c>
       <c r="E78" s="2">
-        <f>-D50</f>
+        <f t="shared" si="8"/>
         <v>-4.0155449999999999E-9</v>
       </c>
       <c r="F78" s="2">
-        <f>-E50</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G78" s="2">
-        <f>-F50</f>
+        <f t="shared" si="8"/>
         <v>1.2386E-7</v>
       </c>
       <c r="H78" s="2">
-        <f>-G50</f>
+        <f t="shared" si="8"/>
         <v>1.3379999999999999E-7</v>
       </c>
     </row>
@@ -24163,31 +24157,31 @@
         <v>2.75</v>
       </c>
       <c r="B79" s="2">
-        <f>-A51</f>
+        <f t="shared" si="8"/>
         <v>-3.1156999999999999E-8</v>
       </c>
       <c r="C79" s="2">
-        <f>-B51</f>
+        <f t="shared" si="8"/>
         <v>2.0353E-8</v>
       </c>
       <c r="D79" s="2">
-        <f>-C51</f>
+        <f t="shared" si="8"/>
         <v>3.6362999999999999E-9</v>
       </c>
       <c r="E79" s="2">
-        <f>-D51</f>
+        <f t="shared" si="8"/>
         <v>-2.4165216666666665E-9</v>
       </c>
       <c r="F79" s="2">
-        <f>-E51</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G79" s="2">
-        <f>-F51</f>
+        <f t="shared" si="8"/>
         <v>-3.1156999999999999E-8</v>
       </c>
       <c r="H79" s="2">
-        <f>-G51</f>
+        <f t="shared" si="8"/>
         <v>6.9390000000000001E-8</v>
       </c>
     </row>
@@ -24196,31 +24190,31 @@
         <v>2.875</v>
       </c>
       <c r="B80" s="2">
-        <f>-A52</f>
+        <f t="shared" si="8"/>
         <v>-3.6876E-9</v>
       </c>
       <c r="C80" s="2">
-        <f>-B52</f>
+        <f t="shared" si="8"/>
         <v>4.5750000000000003E-8</v>
       </c>
       <c r="D80" s="2">
-        <f>-C52</f>
+        <f t="shared" si="8"/>
         <v>2.7233833333333339E-9</v>
       </c>
       <c r="E80" s="2">
-        <f>-D52</f>
+        <f t="shared" si="8"/>
         <v>-2.3133216666666679E-9</v>
       </c>
       <c r="F80" s="2">
-        <f>-E52</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G80" s="2">
-        <f>-F52</f>
+        <f t="shared" si="8"/>
         <v>-3.6876E-9</v>
       </c>
       <c r="H80" s="2">
-        <f>-G52</f>
+        <f t="shared" si="8"/>
         <v>1.536E-8</v>
       </c>
     </row>
@@ -24229,31 +24223,31 @@
         <v>3</v>
       </c>
       <c r="B81" s="2">
-        <f>-A53</f>
+        <f t="shared" si="8"/>
         <v>1.2715E-8</v>
       </c>
       <c r="C81" s="2">
-        <f>-B53</f>
+        <f t="shared" si="8"/>
         <v>8.1841500000000005E-9</v>
       </c>
       <c r="D81" s="2">
-        <f>-C53</f>
+        <f t="shared" si="8"/>
         <v>2.3391949999999996E-9</v>
       </c>
       <c r="E81" s="2">
-        <f>-D53</f>
+        <f t="shared" si="8"/>
         <v>-4.4602916666666669E-10</v>
       </c>
       <c r="F81" s="2">
-        <f>-E53</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="G81" s="2">
-        <f>-F53</f>
+        <f t="shared" si="8"/>
         <v>1.2715E-8</v>
       </c>
       <c r="H81" s="2">
-        <f>-G53</f>
+        <f t="shared" si="8"/>
         <v>7.7383999999999997E-9</v>
       </c>
     </row>

</xml_diff>